<commit_message>
update demographics food security and poverty, and link to target pop
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Aug02/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Aug02/InputForCode_Bangladesh.xlsx
@@ -961,6 +961,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1289,7 +1340,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3248,7 +3299,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add to demographics sheet: fraction food insecure (not poor)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Aug02/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Aug02/InputForCode_Bangladesh.xlsx
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="80">
   <si>
     <t>indicators</t>
   </si>
@@ -493,16 +493,18 @@
   </si>
   <si>
     <t>fraction food insecure (poor)</t>
+  </si>
+  <si>
+    <t>fraction food insecure (not poor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -674,7 +676,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -977,6 +979,57 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1337,15 +1390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+      <selection activeCell="B7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1384,7 +1437,7 @@
       <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="13">
         <v>0.56799999999999995</v>
       </c>
     </row>
@@ -1394,6 +1447,14 @@
       </c>
       <c r="B6" s="26">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="26">
+        <v>0.20599999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiply affected fraction with fraction poor (target) for balanced energy supplements
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Aug02/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Aug02/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500" firstSheet="19" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -1065,6 +1065,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1392,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3360,7 +3411,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3670,8 +3721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3724,16 +3775,15 @@
         <v>76</v>
       </c>
       <c r="C3" s="23">
-        <f>demographics!$B$5</f>
-        <v>0.56799999999999995</v>
+        <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
+        <v>0.22719999999999999</v>
       </c>
       <c r="D3" s="23">
-        <f>demographics!$B$5</f>
-        <v>0.56799999999999995</v>
+        <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
+        <v>0.22719999999999999</v>
       </c>
       <c r="E3" s="23">
-        <f>demographics!$B$5</f>
-        <v>0.56799999999999995</v>
+        <v>0</v>
       </c>
       <c r="F3" s="23">
         <v>0</v>
@@ -3770,7 +3820,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="23">
         <v>0</v>

</xml_diff>